<commit_message>
ApachePOI - excel _write new file
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/WriteInTheExcelFile.xlsx
+++ b/src/test/java/ApachePOI/resource/WriteInTheExcelFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
   <si>
     <t>Merhaba Dünya</t>
   </si>
@@ -345,7 +345,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -358,6 +358,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>